<commit_message>
pushing all the data wrangling i should have pushed ages ago
</commit_message>
<xml_diff>
--- a/extraction/lichen dataset/lichen_nonusable_data.xlsx
+++ b/extraction/lichen dataset/lichen_nonusable_data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretslein/lichen/extraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretslein/lichen/extraction/lichen dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2469B2AC-1257-9F4F-9ABB-2D8B55B85252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B695FB69-3AF0-2E46-B99E-3CDF134C3A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16140" xr2:uid="{4ACB8208-C5EA-C743-ABBD-E40595E24DF5}"/>
+    <workbookView xWindow="7720" yWindow="500" windowWidth="27640" windowHeight="16140" activeTab="1" xr2:uid="{4ACB8208-C5EA-C743-ABBD-E40595E24DF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="24march25" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3769" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4275" uniqueCount="111">
   <si>
     <t>study_id</t>
   </si>
@@ -260,6 +261,114 @@
   <si>
     <t>respiration</t>
   </si>
+  <si>
+    <t>umol CO2 *g^-1 *s^-1</t>
+  </si>
+  <si>
+    <t>co2</t>
+  </si>
+  <si>
+    <t>umol</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>umol *m^-2 *s^-1</t>
+  </si>
+  <si>
+    <t>npp</t>
+  </si>
+  <si>
+    <t>antarctic</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>cyanobacteria</t>
+  </si>
+  <si>
+    <t>green algae</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>insarov1996</t>
+  </si>
+  <si>
+    <t>kappen_1988</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>alectoria</t>
+  </si>
+  <si>
+    <t>ochroleuca</t>
+  </si>
+  <si>
+    <t>net photosynthesis rate</t>
+  </si>
+  <si>
+    <t>mg CO2 *g dry wt ^-1 * hr^-1</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location </t>
+  </si>
+  <si>
+    <t>canada</t>
+  </si>
+  <si>
+    <t>temperate</t>
+  </si>
+  <si>
+    <t>arctic</t>
+  </si>
+  <si>
+    <t>lange_1969</t>
+  </si>
+  <si>
+    <t>ramalina</t>
+  </si>
+  <si>
+    <t>maciformis</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>israel</t>
+  </si>
+  <si>
+    <t>thamnolia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vermicularis </t>
+  </si>
+  <si>
+    <t>europe</t>
+  </si>
+  <si>
+    <t>kappen_1995</t>
+  </si>
+  <si>
+    <t>usnea</t>
+  </si>
+  <si>
+    <t>antarctica</t>
+  </si>
 </sst>
 </file>
 
@@ -315,9 +424,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -355,7 +464,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -461,7 +570,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -603,7 +712,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -613,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3843665A-6476-F945-BA89-D583BCF376BB}">
   <dimension ref="A1:S349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A329" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:O349"/>
     </sheetView>
   </sheetViews>
@@ -16110,4 +16219,2159 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D734F0-FC65-8344-B91A-E5A887E2B90E}">
+  <dimension ref="A2:AH24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2">
+        <v>1.91304348</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q2">
+        <v>0.52173913000000005</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2">
+        <v>3</v>
+      </c>
+      <c r="T2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2">
+        <v>500</v>
+      </c>
+      <c r="AA2">
+        <v>500</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE2">
+        <v>-62</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3">
+        <v>2.1449275399999999</v>
+      </c>
+      <c r="L3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3" t="s">
+        <v>78</v>
+      </c>
+      <c r="P3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3">
+        <v>0.21739130000000001</v>
+      </c>
+      <c r="R3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" t="s">
+        <v>28</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3">
+        <v>500</v>
+      </c>
+      <c r="AA3">
+        <v>500</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE3">
+        <v>-62</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4">
+        <v>1.91304348</v>
+      </c>
+      <c r="L4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N4" t="s">
+        <v>77</v>
+      </c>
+      <c r="O4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q4">
+        <v>1.02898551</v>
+      </c>
+      <c r="R4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4">
+        <v>500</v>
+      </c>
+      <c r="AA4">
+        <v>500</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE4">
+        <v>-62</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5">
+        <v>0.75362319</v>
+      </c>
+      <c r="L5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q5">
+        <v>0.31884057999999998</v>
+      </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U5" t="s">
+        <v>28</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5">
+        <v>500</v>
+      </c>
+      <c r="AA5">
+        <v>500</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE5">
+        <v>-62</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6">
+        <v>0.92753622999999996</v>
+      </c>
+      <c r="L6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q6">
+        <v>0.92753622999999996</v>
+      </c>
+      <c r="R6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="T6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U6" t="s">
+        <v>28</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6">
+        <v>500</v>
+      </c>
+      <c r="AA6">
+        <v>500</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE6">
+        <v>-62</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7">
+        <v>-0.81159420000000004</v>
+      </c>
+      <c r="L7" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7">
+        <v>0.39130435000000002</v>
+      </c>
+      <c r="R7" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+      <c r="T7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U7" t="s">
+        <v>28</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z7">
+        <v>500</v>
+      </c>
+      <c r="AA7">
+        <v>500</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE7">
+        <v>-62</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8">
+        <v>1.2753623199999999</v>
+      </c>
+      <c r="L8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" t="s">
+        <v>78</v>
+      </c>
+      <c r="P8" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q8">
+        <v>0.23188406</v>
+      </c>
+      <c r="R8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+      <c r="T8" t="s">
+        <v>27</v>
+      </c>
+      <c r="U8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z8">
+        <v>500</v>
+      </c>
+      <c r="AA8">
+        <v>500</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE8">
+        <v>-62</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9">
+        <v>1.5652173899999999</v>
+      </c>
+      <c r="L9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" t="s">
+        <v>77</v>
+      </c>
+      <c r="O9" t="s">
+        <v>78</v>
+      </c>
+      <c r="P9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q9">
+        <v>0.53623187999999999</v>
+      </c>
+      <c r="R9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9">
+        <v>3</v>
+      </c>
+      <c r="T9" t="s">
+        <v>27</v>
+      </c>
+      <c r="U9" t="s">
+        <v>28</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z9">
+        <v>500</v>
+      </c>
+      <c r="AA9">
+        <v>500</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE9">
+        <v>-62</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10">
+        <v>8.6956519999999995E-2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" t="s">
+        <v>76</v>
+      </c>
+      <c r="N10" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" t="s">
+        <v>78</v>
+      </c>
+      <c r="P10" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q10">
+        <v>0.66666667000000002</v>
+      </c>
+      <c r="R10" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10">
+        <v>3</v>
+      </c>
+      <c r="T10" t="s">
+        <v>27</v>
+      </c>
+      <c r="U10" t="s">
+        <v>28</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z10">
+        <v>500</v>
+      </c>
+      <c r="AA10">
+        <v>500</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE10">
+        <v>-62</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11">
+        <v>-0.78594249999999999</v>
+      </c>
+      <c r="L11" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q11">
+        <v>0.29712460000000002</v>
+      </c>
+      <c r="R11" t="s">
+        <v>35</v>
+      </c>
+      <c r="S11">
+        <v>3</v>
+      </c>
+      <c r="T11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE11">
+        <v>-62</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12">
+        <v>-1.9361022000000001</v>
+      </c>
+      <c r="L12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" t="s">
+        <v>77</v>
+      </c>
+      <c r="O12" t="s">
+        <v>78</v>
+      </c>
+      <c r="P12" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q12">
+        <v>0.13418530000000001</v>
+      </c>
+      <c r="R12" t="s">
+        <v>35</v>
+      </c>
+      <c r="S12">
+        <v>3</v>
+      </c>
+      <c r="T12" t="s">
+        <v>27</v>
+      </c>
+      <c r="U12" t="s">
+        <v>28</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE12">
+        <v>-62</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13">
+        <v>-2.4728435000000002</v>
+      </c>
+      <c r="L13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13" t="s">
+        <v>78</v>
+      </c>
+      <c r="P13" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q13">
+        <v>0.84345048</v>
+      </c>
+      <c r="R13" t="s">
+        <v>35</v>
+      </c>
+      <c r="S13">
+        <v>3</v>
+      </c>
+      <c r="T13" t="s">
+        <v>27</v>
+      </c>
+      <c r="U13" t="s">
+        <v>28</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE13">
+        <v>-62</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14">
+        <v>-0.40255590000000002</v>
+      </c>
+      <c r="L14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" t="s">
+        <v>77</v>
+      </c>
+      <c r="O14" t="s">
+        <v>78</v>
+      </c>
+      <c r="P14" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q14">
+        <v>0.14376997</v>
+      </c>
+      <c r="R14" t="s">
+        <v>35</v>
+      </c>
+      <c r="S14">
+        <v>3</v>
+      </c>
+      <c r="T14" t="s">
+        <v>27</v>
+      </c>
+      <c r="U14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE14">
+        <v>-62</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15">
+        <v>-0.97763580000000005</v>
+      </c>
+      <c r="L15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" t="s">
+        <v>76</v>
+      </c>
+      <c r="N15" t="s">
+        <v>77</v>
+      </c>
+      <c r="O15" t="s">
+        <v>78</v>
+      </c>
+      <c r="P15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q15">
+        <v>0.32587859000000002</v>
+      </c>
+      <c r="R15" t="s">
+        <v>35</v>
+      </c>
+      <c r="S15">
+        <v>3</v>
+      </c>
+      <c r="T15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U15" t="s">
+        <v>28</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE15">
+        <v>-62</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16">
+        <v>-3.1054312999999998</v>
+      </c>
+      <c r="L16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" t="s">
+        <v>76</v>
+      </c>
+      <c r="N16" t="s">
+        <v>77</v>
+      </c>
+      <c r="O16" t="s">
+        <v>78</v>
+      </c>
+      <c r="P16" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q16">
+        <v>1.5335463300000001</v>
+      </c>
+      <c r="R16" t="s">
+        <v>35</v>
+      </c>
+      <c r="S16">
+        <v>3</v>
+      </c>
+      <c r="T16" t="s">
+        <v>27</v>
+      </c>
+      <c r="U16" t="s">
+        <v>28</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE16">
+        <v>-62</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17">
+        <v>-0.86261980000000005</v>
+      </c>
+      <c r="L17" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" t="s">
+        <v>76</v>
+      </c>
+      <c r="N17" t="s">
+        <v>77</v>
+      </c>
+      <c r="O17" t="s">
+        <v>78</v>
+      </c>
+      <c r="P17" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q17">
+        <v>0.23961661000000001</v>
+      </c>
+      <c r="R17" t="s">
+        <v>35</v>
+      </c>
+      <c r="S17">
+        <v>3</v>
+      </c>
+      <c r="T17" t="s">
+        <v>27</v>
+      </c>
+      <c r="U17" t="s">
+        <v>28</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE17">
+        <v>-62</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K18">
+        <v>-3.4696486000000002</v>
+      </c>
+      <c r="L18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" t="s">
+        <v>76</v>
+      </c>
+      <c r="N18" t="s">
+        <v>77</v>
+      </c>
+      <c r="O18" t="s">
+        <v>78</v>
+      </c>
+      <c r="P18" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q18">
+        <v>0.11501597</v>
+      </c>
+      <c r="R18" t="s">
+        <v>35</v>
+      </c>
+      <c r="S18">
+        <v>3</v>
+      </c>
+      <c r="T18" t="s">
+        <v>27</v>
+      </c>
+      <c r="U18" t="s">
+        <v>28</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE18">
+        <v>-62</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19">
+        <v>23</v>
+      </c>
+      <c r="I19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K19">
+        <v>-4.9265176000000004</v>
+      </c>
+      <c r="L19" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N19" t="s">
+        <v>77</v>
+      </c>
+      <c r="O19" t="s">
+        <v>78</v>
+      </c>
+      <c r="P19" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q19">
+        <v>0.94888178999999995</v>
+      </c>
+      <c r="R19" t="s">
+        <v>35</v>
+      </c>
+      <c r="S19">
+        <v>3</v>
+      </c>
+      <c r="T19" t="s">
+        <v>27</v>
+      </c>
+      <c r="U19" t="s">
+        <v>28</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE19">
+        <v>-62</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20">
+        <v>7</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20">
+        <v>0.33</v>
+      </c>
+      <c r="L20" t="s">
+        <v>93</v>
+      </c>
+      <c r="M20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N20" t="s">
+        <v>94</v>
+      </c>
+      <c r="O20" t="s">
+        <v>78</v>
+      </c>
+      <c r="P20" t="s">
+        <v>95</v>
+      </c>
+      <c r="T20" t="s">
+        <v>27</v>
+      </c>
+      <c r="U20" t="s">
+        <v>28</v>
+      </c>
+      <c r="X20" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z20">
+        <v>150</v>
+      </c>
+      <c r="AA20">
+        <v>150</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE20">
+        <v>57</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21">
+        <v>0.08</v>
+      </c>
+      <c r="L21" t="s">
+        <v>93</v>
+      </c>
+      <c r="M21" t="s">
+        <v>76</v>
+      </c>
+      <c r="N21" t="s">
+        <v>94</v>
+      </c>
+      <c r="O21" t="s">
+        <v>78</v>
+      </c>
+      <c r="P21" t="s">
+        <v>95</v>
+      </c>
+      <c r="T21" t="s">
+        <v>27</v>
+      </c>
+      <c r="U21" t="s">
+        <v>28</v>
+      </c>
+      <c r="X21" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z21">
+        <v>150</v>
+      </c>
+      <c r="AA21">
+        <v>150</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE21">
+        <v>75</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22">
+        <v>20</v>
+      </c>
+      <c r="I22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22" t="s">
+        <v>93</v>
+      </c>
+      <c r="M22" t="s">
+        <v>76</v>
+      </c>
+      <c r="N22" t="s">
+        <v>94</v>
+      </c>
+      <c r="O22" t="s">
+        <v>78</v>
+      </c>
+      <c r="P22" t="s">
+        <v>95</v>
+      </c>
+      <c r="T22" t="s">
+        <v>27</v>
+      </c>
+      <c r="U22" t="s">
+        <v>28</v>
+      </c>
+      <c r="X22" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z22">
+        <v>700</v>
+      </c>
+      <c r="AA22">
+        <v>700</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE22">
+        <v>30.7944</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23">
+        <v>1.17</v>
+      </c>
+      <c r="L23" t="s">
+        <v>93</v>
+      </c>
+      <c r="M23" t="s">
+        <v>76</v>
+      </c>
+      <c r="N23" t="s">
+        <v>94</v>
+      </c>
+      <c r="O23" t="s">
+        <v>78</v>
+      </c>
+      <c r="P23" t="s">
+        <v>95</v>
+      </c>
+      <c r="T23" t="s">
+        <v>27</v>
+      </c>
+      <c r="U23" t="s">
+        <v>28</v>
+      </c>
+      <c r="X23" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z23">
+        <v>260</v>
+      </c>
+      <c r="AA23">
+        <v>260</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE23">
+        <v>54.526000000000003</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24">
+        <v>13</v>
+      </c>
+      <c r="I24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24">
+        <v>0.3</v>
+      </c>
+      <c r="L24" t="s">
+        <v>93</v>
+      </c>
+      <c r="M24" t="s">
+        <v>76</v>
+      </c>
+      <c r="N24" t="s">
+        <v>94</v>
+      </c>
+      <c r="O24" t="s">
+        <v>78</v>
+      </c>
+      <c r="P24" t="s">
+        <v>95</v>
+      </c>
+      <c r="T24" t="s">
+        <v>27</v>
+      </c>
+      <c r="U24" t="s">
+        <v>28</v>
+      </c>
+      <c r="X24" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z24">
+        <v>600</v>
+      </c>
+      <c r="AA24">
+        <v>600</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE24">
+        <v>-82.862799999999993</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>